<commit_message>
upload full scan and peak shape files
</commit_message>
<xml_diff>
--- a/inst/gui/default_settings.xlsx
+++ b/inst/gui/default_settings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="116">
   <si>
     <t>Variable</t>
   </si>
@@ -274,9 +274,6 @@
     <t>Intensity on middle cup at mass 18 with split in, BF off</t>
   </si>
   <si>
-    <t>Full scan complete and uploaded?</t>
-  </si>
-  <si>
     <t>nitrogen</t>
   </si>
   <si>
@@ -359,6 +356,18 @@
   </si>
   <si>
     <t>Deflection</t>
+  </si>
+  <si>
+    <t>Full scan complete and file selected?</t>
+  </si>
+  <si>
+    <t>peak_shape</t>
+  </si>
+  <si>
+    <t>Peak shape scan complete &amp; selected?</t>
+  </si>
+  <si>
+    <t>Run a peak shape scan (from ? To ?), split out, BF on</t>
   </si>
 </sst>
 </file>
@@ -415,8 +424,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -493,7 +508,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -529,6 +544,9 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -564,6 +582,9 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1038,17 +1059,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D25" sqref="D25:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="56.83203125" bestFit="1" customWidth="1"/>
@@ -1176,7 +1197,7 @@
         <v>78</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>37</v>
@@ -1479,10 +1500,10 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
         <v>85</v>
-      </c>
-      <c r="C20" t="s">
-        <v>86</v>
       </c>
       <c r="D20" t="s">
         <v>60</v>
@@ -1491,7 +1512,7 @@
         <v>37</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1499,13 +1520,13 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>7</v>
@@ -1514,7 +1535,7 @@
         <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1522,13 +1543,13 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>7</v>
@@ -1537,133 +1558,193 @@
         <v>26</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>96</v>
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" t="s">
+        <v>114</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>98</v>
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" t="s">
+        <v>114</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>101</v>
+        <v>37</v>
+      </c>
+      <c r="G24" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>104</v>
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
+        <v>114</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>105</v>
+        <v>37</v>
+      </c>
+      <c r="G25" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>